<commit_message>
Update sample data defintions with better grocery figure
</commit_message>
<xml_diff>
--- a/YoFi.Tests/SampleData/FullSampleDataDefinition.xlsx
+++ b/YoFi.Tests/SampleData/FullSampleDataDefinition.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\jcoliz\Ofx\SampleData\SampleGen.Test\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\jcoliz\Ofx\YoFi.Tests\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51CD24A-3E1C-4EF9-B462-28A793229AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD8DEC0-4323-4DA4-AD0C-E5417C12276D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6130" yWindow="3350" windowWidth="28800" windowHeight="15460" xr2:uid="{D78380F0-A539-4D8B-9BEC-B3C0621EF4A6}"/>
+    <workbookView xWindow="6470" yWindow="3690" windowWidth="28800" windowHeight="15460" xr2:uid="{D78380F0-A539-4D8B-9BEC-B3C0621EF4A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Definition" sheetId="1" r:id="rId1"/>
@@ -723,7 +723,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1040,8 +1040,8 @@
         <v>72</v>
       </c>
       <c r="C15" s="1">
-        <f>-350*52</f>
-        <v>-18200</v>
+        <f>-85*52</f>
+        <v>-4420</v>
       </c>
       <c r="D15" t="s">
         <v>16</v>
@@ -1412,276 +1412,276 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C33" s="1">
-        <v>120000</v>
+        <v>25000</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>11</v>
       </c>
       <c r="E33" t="s">
         <v>13</v>
       </c>
       <c r="F33" t="s">
         <v>13</v>
-      </c>
-      <c r="G33" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="1">
+        <v>120000</v>
+      </c>
+      <c r="D34" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C35" s="1">
         <f>4000</f>
         <v>4000</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>76</v>
       </c>
-      <c r="E34" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="E35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C36" s="1">
         <f>-687*24</f>
         <v>-16488</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>76</v>
       </c>
-      <c r="E35" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="E36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C37" s="1">
         <f>-310*24</f>
         <v>-7440</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>76</v>
       </c>
-      <c r="E36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" t="s">
+      <c r="E37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C38" s="1">
         <f>-73*24</f>
         <v>-1752</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>76</v>
       </c>
-      <c r="E37" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" t="s">
+      <c r="E38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C39" s="1">
         <f>-260*24</f>
         <v>-6240</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>76</v>
       </c>
-      <c r="E38" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" t="s">
+      <c r="E39" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C40" s="1">
         <f>-48*24</f>
         <v>-1152</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>76</v>
       </c>
-      <c r="E39" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" t="s">
+      <c r="E40" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C41" s="1">
         <f>-500*12</f>
         <v>-6000</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>76</v>
       </c>
-      <c r="E40" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" t="s">
-        <v>13</v>
-      </c>
-      <c r="G40" t="s">
+      <c r="E41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C42" s="1">
         <f>-4000</f>
         <v>-4000</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>76</v>
       </c>
-      <c r="E41" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" t="s">
-        <v>13</v>
-      </c>
-      <c r="G41" t="s">
+      <c r="E42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C43" s="1">
         <f>-19000</f>
         <v>-19000</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>76</v>
       </c>
-      <c r="E42" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" t="s">
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C44" s="1">
         <f>-200</f>
         <v>-200</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>76</v>
       </c>
-      <c r="E43" t="s">
-        <v>13</v>
-      </c>
-      <c r="F43" t="s">
-        <v>13</v>
-      </c>
-      <c r="G43" t="s">
+      <c r="E44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C45" s="1">
         <f>-50</f>
         <v>-50</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>76</v>
       </c>
-      <c r="E44" t="s">
-        <v>13</v>
-      </c>
-      <c r="F44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" t="s">
+      <c r="E45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>40</v>
-      </c>
-      <c r="B45" t="s">
-        <v>85</v>
-      </c>
-      <c r="C45" s="1">
-        <v>25000</v>
-      </c>
-      <c r="D45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" t="s">
-        <v>13</v>
-      </c>
-      <c r="F45" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>